<commit_message>
02/05/2023 - Automatic Set & Advanced Flow (D0952)
Se realizó las pruebas para UI
</commit_message>
<xml_diff>
--- a/Pruebas.xlsx
+++ b/Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\OneDrive\Documents\LR\Area Desarrollo\Devs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15E4884C-B7B9-4FCF-8B63-34EBA3D64484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED03EDD0-ABDF-4D09-81A3-C521C7B42977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5895" yWindow="2850" windowWidth="19200" windowHeight="11505" xr2:uid="{0CE0351C-50CF-4043-9B86-607898032C7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0CE0351C-50CF-4043-9B86-607898032C7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
   <dimension ref="E4:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>